<commit_message>
Github_copilot_cdanastasio_002: aggiornamento file Excel
</commit_message>
<xml_diff>
--- a/prompts/Registro_Prompt_AI.xlsx
+++ b/prompts/Registro_Prompt_AI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.danastasio\Repository_AI\AI_Code_Repository\prompts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F79DB0-A960-4D72-9B20-70C9C7035D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D52884A-9DFE-4BA1-9930-F88A2A5707E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="552" yWindow="12" windowWidth="22764" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regprompt" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="231">
   <si>
     <t>ID Prompt</t>
   </si>
@@ -699,6 +699,32 @@
   </si>
   <si>
     <t>Sì</t>
+  </si>
+  <si>
+    <t>Github_copilot_cdanastasio_002</t>
+  </si>
+  <si>
+    <t>LeMoire</t>
+  </si>
+  <si>
+    <t>Python 3.11.9, pytest</t>
+  </si>
+  <si>
+    <t>PROMPT 1: @workspace/test Genera lo unit test per il file modelli.py usando pytest
+PROMPT 2: Inserisci il test nella cartella 'tests' del progetto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generare unit test per il file modelli.py </t>
+  </si>
+  <si>
+    <t>Sì - Unit test eseguito correttamente</t>
+  </si>
+  <si>
+    <t>Dopo aver inviato i due prompt, il modello ha generato un primo test che è fallito, 
+ma ha provveduto in maniera autonoma alla correzione del test senza la necessità di scrivere ulteriori prompt.</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
   </si>
 </sst>
 </file>
@@ -893,7 +919,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -929,23 +955,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -958,6 +972,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1324,17 +1347,17 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="21" customWidth="1"/>
-    <col min="2" max="8" width="30.88671875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" style="18" customWidth="1"/>
+    <col min="2" max="8" width="30.88671875" style="18" customWidth="1"/>
     <col min="9" max="10" width="20" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="21" customWidth="1"/>
+    <col min="11" max="11" width="20" style="18" customWidth="1"/>
     <col min="12" max="12" width="20" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="20" style="21" customWidth="1"/>
+    <col min="13" max="14" width="20" style="18" customWidth="1"/>
     <col min="15" max="15" width="20" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
     <col min="17" max="17" width="17.21875" bestFit="1" customWidth="1"/>
@@ -1346,40 +1369,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="17" t="s">
+      <c r="R1" s="24"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="18"/>
-      <c r="V1" s="19"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="25"/>
     </row>
     <row r="2" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1388,16 +1411,16 @@
       <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -1426,28 +1449,28 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1456,16 +1479,16 @@
       <c r="J3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -1494,98 +1517,128 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="22">
         <v>45961</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>217</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="17" t="s">
         <v>218</v>
       </c>
       <c r="L4" s="3"/>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="17" t="s">
         <v>220</v>
       </c>
       <c r="O4" s="14"/>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="20" t="s">
         <v>222</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+    <row r="5" spans="1:22" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="22">
+        <v>45965</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>227</v>
+      </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="17" t="s">
+        <v>228</v>
+      </c>
       <c r="L5" s="3"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
+      <c r="M5" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>229</v>
+      </c>
       <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
+      <c r="P5" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="R5" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>222</v>
+      </c>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="24"/>
+      <c r="K6" s="20"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1596,20 +1649,20 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="24"/>
+      <c r="K7" s="20"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -1620,20 +1673,20 @@
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="24"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -1644,20 +1697,20 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="24"/>
+      <c r="K9" s="20"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
@@ -1668,20 +1721,20 @@
       <c r="V9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="24"/>
+      <c r="K10" s="20"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -1692,20 +1745,20 @@
       <c r="V10" s="3"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="24"/>
+      <c r="K11" s="20"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1716,20 +1769,20 @@
       <c r="V11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="24"/>
+      <c r="K12" s="20"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1740,20 +1793,20 @@
       <c r="V12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="24"/>
+      <c r="K13" s="20"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -1764,20 +1817,20 @@
       <c r="V13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="24"/>
+      <c r="K14" s="20"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -1788,20 +1841,20 @@
       <c r="V14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="24"/>
+      <c r="K15" s="20"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -1812,20 +1865,20 @@
       <c r="V15" s="3"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="24"/>
+      <c r="K16" s="20"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -1836,20 +1889,20 @@
       <c r="V16" s="3"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="24"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -1860,20 +1913,20 @@
       <c r="V17" s="3"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="24"/>
+      <c r="K18" s="20"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -1884,20 +1937,20 @@
       <c r="V18" s="3"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="24"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -1908,20 +1961,20 @@
       <c r="V19" s="3"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="24"/>
+      <c r="K20" s="20"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -1932,20 +1985,20 @@
       <c r="V20" s="3"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="24"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -1956,20 +2009,20 @@
       <c r="V21" s="3"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="24"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -1980,20 +2033,20 @@
       <c r="V22" s="3"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="24"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2004,20 +2057,20 @@
       <c r="V23" s="3"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="24"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2028,20 +2081,20 @@
       <c r="V24" s="3"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="24"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2052,20 +2105,20 @@
       <c r="V25" s="3"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="24"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>

</xml_diff>